<commit_message>
Refactor angle calculation and plotting in Lab 2
</commit_message>
<xml_diff>
--- a/Lab_2/Data.xlsx
+++ b/Lab_2/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/kristgg_ntnu_no/Documents/2024 Vår/Sensorer og instrumentering/Lab/Lab_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{33F313D0-C212-4A6D-B5A5-08A222D74031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D82D9319-7C17-4CB7-98CA-85FBED8B5E1B}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="8_{33F313D0-C212-4A6D-B5A5-08A222D74031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51C6DD37-BBD1-416E-B6C3-61779E7C1CDC}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CEA101CB-4BD1-4A33-9525-02A1914AA89A}"/>
   </bookViews>
@@ -85,9 +85,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="166" formatCode="0.00000"/>
-    <numFmt numFmtId="167" formatCode="0.0000"/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -142,36 +142,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -187,6 +177,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -506,18 +500,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED319A0D-C889-4D07-8610-3A79F9BB31F1}">
-  <dimension ref="A1:Y28"/>
+  <dimension ref="A1:Y33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="86" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="11.90625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="4.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="4.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="6.7265625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.54296875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.54296875" bestFit="1" customWidth="1"/>
@@ -536,36 +530,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="14" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="5" t="s">
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
@@ -592,28 +586,28 @@
       <c r="I2" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="N2" t="s">
         <v>9</v>
       </c>
-      <c r="O2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="P2" s="8" t="s">
+      <c r="O2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P2" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" s="12" t="s">
+      <c r="Q2" s="5" t="s">
         <v>12</v>
       </c>
       <c r="R2" t="s">
@@ -669,28 +663,28 @@
       <c r="I3" s="4">
         <v>0.28799999999999998</v>
       </c>
-      <c r="J3" s="16">
+      <c r="J3" s="8">
         <v>58.425171286805202</v>
       </c>
-      <c r="K3" s="18">
+      <c r="K3" s="2">
         <v>1.0197116049963999</v>
       </c>
-      <c r="L3" s="17">
+      <c r="L3" s="9">
         <v>21</v>
       </c>
-      <c r="M3" s="8">
-        <v>10</v>
-      </c>
-      <c r="N3" s="8">
+      <c r="M3">
+        <v>10</v>
+      </c>
+      <c r="N3">
         <v>-11</v>
       </c>
-      <c r="O3" s="10">
+      <c r="O3" s="4">
         <v>0.67199999999999904</v>
       </c>
-      <c r="P3" s="9">
-        <v>0.32</v>
-      </c>
-      <c r="Q3" s="13">
+      <c r="P3" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="Q3" s="6">
         <v>-0.35199999999999998</v>
       </c>
       <c r="R3" s="1">
@@ -746,28 +740,28 @@
       <c r="I4" s="4">
         <v>0.28799999999999998</v>
       </c>
-      <c r="J4" s="16">
+      <c r="J4" s="8">
         <v>56.9017981908368</v>
       </c>
-      <c r="K4" s="18">
+      <c r="K4" s="2">
         <v>0.99312372873545496</v>
       </c>
-      <c r="L4" s="17">
+      <c r="L4" s="9">
         <v>21</v>
       </c>
-      <c r="M4" s="8">
-        <v>10</v>
-      </c>
-      <c r="N4" s="8">
+      <c r="M4">
+        <v>10</v>
+      </c>
+      <c r="N4">
         <v>-12</v>
       </c>
-      <c r="O4" s="10">
+      <c r="O4" s="4">
         <v>0.67199999999999904</v>
       </c>
-      <c r="P4" s="9">
-        <v>0.32</v>
-      </c>
-      <c r="Q4" s="13">
+      <c r="P4" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="Q4" s="6">
         <v>-0.38400000000000001</v>
       </c>
       <c r="R4" s="1">
@@ -823,28 +817,28 @@
       <c r="I5" s="1">
         <v>0.32</v>
       </c>
-      <c r="J5" s="16">
+      <c r="J5" s="8">
         <v>58.425171286805202</v>
       </c>
-      <c r="K5" s="18">
+      <c r="K5" s="2">
         <v>1.0197116049963999</v>
       </c>
-      <c r="L5" s="17">
+      <c r="L5" s="9">
         <v>21</v>
       </c>
-      <c r="M5" s="8">
-        <v>10</v>
-      </c>
-      <c r="N5" s="8">
+      <c r="M5">
+        <v>10</v>
+      </c>
+      <c r="N5">
         <v>-11</v>
       </c>
-      <c r="O5" s="10">
+      <c r="O5" s="4">
         <v>0.67199999999999904</v>
       </c>
-      <c r="P5" s="9">
-        <v>0.32</v>
-      </c>
-      <c r="Q5" s="13">
+      <c r="P5" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="Q5" s="6">
         <v>-0.35199999999999998</v>
       </c>
       <c r="R5" s="1">
@@ -900,28 +894,28 @@
       <c r="I6" s="1">
         <v>0.32</v>
       </c>
-      <c r="J6" s="16">
+      <c r="J6" s="8">
         <v>58.425171286805202</v>
       </c>
-      <c r="K6" s="18">
+      <c r="K6" s="2">
         <v>1.0197116049963999</v>
       </c>
-      <c r="L6" s="17">
+      <c r="L6" s="9">
         <v>21</v>
       </c>
-      <c r="M6" s="8">
-        <v>10</v>
-      </c>
-      <c r="N6" s="19">
+      <c r="M6">
+        <v>10</v>
+      </c>
+      <c r="N6">
         <v>-11</v>
       </c>
-      <c r="O6" s="10">
+      <c r="O6" s="4">
         <v>0.67199999999999904</v>
       </c>
-      <c r="P6" s="9">
-        <v>0.32</v>
-      </c>
-      <c r="Q6" s="13">
+      <c r="P6" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="Q6" s="6">
         <v>-0.35199999999999998</v>
       </c>
       <c r="R6" s="1">
@@ -977,28 +971,28 @@
       <c r="I7" s="1">
         <v>0.32</v>
       </c>
-      <c r="J7" s="16">
+      <c r="J7" s="8">
         <v>58.425171286805202</v>
       </c>
-      <c r="K7" s="18">
+      <c r="K7" s="2">
         <v>1.0197116049963999</v>
       </c>
-      <c r="L7" s="17">
+      <c r="L7" s="9">
         <v>21</v>
       </c>
-      <c r="M7" s="8">
-        <v>10</v>
-      </c>
-      <c r="N7" s="19">
+      <c r="M7">
+        <v>10</v>
+      </c>
+      <c r="N7">
         <v>-11</v>
       </c>
-      <c r="O7" s="10">
+      <c r="O7" s="4">
         <v>0.67199999999999904</v>
       </c>
-      <c r="P7" s="9">
-        <v>0.32</v>
-      </c>
-      <c r="Q7" s="13">
+      <c r="P7" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="Q7" s="6">
         <v>-0.35199999999999998</v>
       </c>
       <c r="R7" s="1">
@@ -1054,28 +1048,28 @@
       <c r="I8" s="1">
         <v>0.32</v>
       </c>
-      <c r="J8" s="16">
+      <c r="J8" s="8">
         <v>58.4736042675463</v>
       </c>
-      <c r="K8" s="18">
+      <c r="K8" s="2">
         <v>1.02055691997689</v>
       </c>
-      <c r="L8" s="17">
+      <c r="L8" s="9">
         <v>22</v>
       </c>
-      <c r="M8" s="8">
-        <v>10</v>
-      </c>
-      <c r="N8" s="19">
+      <c r="M8">
+        <v>10</v>
+      </c>
+      <c r="N8">
         <v>-11</v>
       </c>
-      <c r="O8" s="10">
+      <c r="O8" s="4">
         <v>0.70399999999999996</v>
       </c>
-      <c r="P8" s="9">
-        <v>0.32</v>
-      </c>
-      <c r="Q8" s="13">
+      <c r="P8" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="Q8" s="6">
         <v>-0.35199999999999998</v>
       </c>
       <c r="R8" s="1">
@@ -1131,28 +1125,28 @@
       <c r="I9" s="1">
         <v>0.32</v>
       </c>
-      <c r="J9" s="16">
+      <c r="J9" s="8">
         <v>56.9017981908368</v>
       </c>
-      <c r="K9" s="18">
+      <c r="K9" s="2">
         <v>0.99312372873545496</v>
       </c>
-      <c r="L9" s="17">
+      <c r="L9" s="9">
         <v>21</v>
       </c>
-      <c r="M9" s="8">
-        <v>10</v>
-      </c>
-      <c r="N9" s="19">
+      <c r="M9">
+        <v>10</v>
+      </c>
+      <c r="N9">
         <v>-12</v>
       </c>
-      <c r="O9" s="10">
+      <c r="O9" s="4">
         <v>0.67199999999999904</v>
       </c>
-      <c r="P9" s="9">
-        <v>0.32</v>
-      </c>
-      <c r="Q9" s="13">
+      <c r="P9" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="Q9" s="6">
         <v>-0.38400000000000001</v>
       </c>
       <c r="R9" s="1">
@@ -1208,28 +1202,28 @@
       <c r="I10" s="1">
         <v>0.32</v>
       </c>
-      <c r="J10" s="16">
+      <c r="J10" s="8">
         <v>56.9017981908368</v>
       </c>
-      <c r="K10" s="18">
+      <c r="K10" s="2">
         <v>0.99312372873545496</v>
       </c>
-      <c r="L10" s="17">
+      <c r="L10" s="9">
         <v>21</v>
       </c>
-      <c r="M10" s="8">
-        <v>10</v>
-      </c>
-      <c r="N10" s="19">
+      <c r="M10">
+        <v>10</v>
+      </c>
+      <c r="N10">
         <v>-12</v>
       </c>
-      <c r="O10" s="10">
+      <c r="O10" s="4">
         <v>0.67199999999999904</v>
       </c>
-      <c r="P10" s="9">
-        <v>0.32</v>
-      </c>
-      <c r="Q10" s="13">
+      <c r="P10" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="Q10" s="6">
         <v>-0.38400000000000001</v>
       </c>
       <c r="R10" s="1">
@@ -1285,28 +1279,28 @@
       <c r="I11" s="1">
         <v>0.32</v>
       </c>
-      <c r="J11" s="16">
+      <c r="J11" s="8">
         <v>58.425171286805202</v>
       </c>
-      <c r="K11" s="18">
+      <c r="K11" s="2">
         <v>1.0197116049963999</v>
       </c>
-      <c r="L11" s="17">
+      <c r="L11" s="9">
         <v>21</v>
       </c>
-      <c r="M11" s="8">
-        <v>10</v>
-      </c>
-      <c r="N11" s="19">
+      <c r="M11">
+        <v>10</v>
+      </c>
+      <c r="N11">
         <v>-11</v>
       </c>
-      <c r="O11" s="10">
+      <c r="O11" s="4">
         <v>0.67199999999999904</v>
       </c>
-      <c r="P11" s="9">
-        <v>0.32</v>
-      </c>
-      <c r="Q11" s="13">
+      <c r="P11" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="Q11" s="6">
         <v>-0.35199999999999998</v>
       </c>
       <c r="R11" s="1">
@@ -1362,28 +1356,28 @@
       <c r="I12" s="1">
         <v>0.32</v>
       </c>
-      <c r="J12" s="16">
+      <c r="J12" s="8">
         <v>58.425171286805202</v>
       </c>
-      <c r="K12" s="18">
+      <c r="K12" s="2">
         <v>1.0197116049963999</v>
       </c>
-      <c r="L12" s="17">
+      <c r="L12" s="9">
         <v>21</v>
       </c>
-      <c r="M12" s="8">
-        <v>10</v>
-      </c>
-      <c r="N12" s="19">
+      <c r="M12">
+        <v>10</v>
+      </c>
+      <c r="N12">
         <v>-11</v>
       </c>
-      <c r="O12" s="10">
+      <c r="O12" s="4">
         <v>0.67199999999999904</v>
       </c>
-      <c r="P12" s="9">
-        <v>0.32</v>
-      </c>
-      <c r="Q12" s="13">
+      <c r="P12" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="Q12" s="6">
         <v>-0.35199999999999998</v>
       </c>
       <c r="R12" s="1">
@@ -1420,7 +1414,7 @@
         <v>1.0112517005192607</v>
       </c>
       <c r="C14">
-        <f t="shared" ref="C14:Y14" si="0">_xlfn.STDEV.P(C3:C12)</f>
+        <f t="shared" ref="C14:S14" si="0">_xlfn.STDEV.P(C3:C12)</f>
         <v>1.7649671740448975E-2</v>
       </c>
       <c r="J14">
@@ -1449,7 +1443,7 @@
         <v>1.0226300018030965</v>
       </c>
       <c r="C15">
-        <f t="shared" ref="C15:Y15" si="1">_xlfn.VAR.P(C3:C12)</f>
+        <f t="shared" ref="C15:S15" si="1">_xlfn.VAR.P(C3:C12)</f>
         <v>3.1151091254560313E-4</v>
       </c>
       <c r="J15">
@@ -1481,15 +1475,15 @@
         <f t="shared" ref="C16:Y16" si="2">MEDIAN(C3:C12)</f>
         <v>4.2162761509865803</v>
       </c>
-      <c r="D16" s="20">
+      <c r="D16" s="9">
         <f t="shared" si="2"/>
         <v>-21</v>
       </c>
-      <c r="E16" s="20">
+      <c r="E16" s="9">
         <f t="shared" si="2"/>
         <v>-11</v>
       </c>
-      <c r="F16" s="20">
+      <c r="F16" s="9">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
@@ -1513,15 +1507,15 @@
         <f t="shared" si="2"/>
         <v>1.0197116049963999</v>
       </c>
-      <c r="L16" s="20">
+      <c r="L16" s="9">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="M16" s="20">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="N16" s="20">
+      <c r="M16" s="9">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="N16" s="9">
         <f t="shared" si="2"/>
         <v>-11</v>
       </c>
@@ -1545,15 +1539,15 @@
         <f t="shared" si="2"/>
         <v>3.099492041745795</v>
       </c>
-      <c r="T16" s="20">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="U16" s="20">
+      <c r="T16" s="9">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="U16" s="9">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="V16" s="20">
+      <c r="V16" s="9">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
@@ -1570,55 +1564,160 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="17" spans="8:15" x14ac:dyDescent="0.35">
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-    </row>
-    <row r="19" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="6:12" x14ac:dyDescent="0.35">
       <c r="H19" s="1"/>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="6:12" x14ac:dyDescent="0.35">
       <c r="H20" s="1"/>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="6:12" x14ac:dyDescent="0.35">
       <c r="H21" s="1"/>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="6:12" x14ac:dyDescent="0.35">
       <c r="H22" s="1"/>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="6:12" x14ac:dyDescent="0.35">
       <c r="H23" s="1"/>
       <c r="L23" s="1"/>
     </row>
-    <row r="24" spans="8:15" x14ac:dyDescent="0.35">
-      <c r="H24" s="1"/>
+    <row r="24" spans="6:12" x14ac:dyDescent="0.35">
+      <c r="F24" s="1">
+        <f>B3</f>
+        <v>243.19793959904899</v>
+      </c>
+      <c r="G24" s="1">
+        <v>242.77652220312299</v>
+      </c>
+      <c r="H24" s="1">
+        <f>F24-G24</f>
+        <v>0.42141739592599947</v>
+      </c>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="8:15" x14ac:dyDescent="0.35">
-      <c r="H25" s="1"/>
+    <row r="25" spans="6:12" x14ac:dyDescent="0.35">
+      <c r="F25" s="1">
+        <f t="shared" ref="F25:F33" si="3">B4</f>
+        <v>244.71500395394801</v>
+      </c>
+      <c r="G25" s="1">
+        <v>243.12254901112601</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" ref="H25:H33" si="4">F25-G25</f>
+        <v>1.5924549428220018</v>
+      </c>
       <c r="L25" s="1"/>
     </row>
-    <row r="26" spans="8:15" x14ac:dyDescent="0.35">
-      <c r="H26" s="1"/>
+    <row r="26" spans="6:12" x14ac:dyDescent="0.35">
+      <c r="F26" s="1">
+        <f t="shared" si="3"/>
+        <v>241.57482871319399</v>
+      </c>
+      <c r="G26" s="1">
+        <v>242.76547756824999</v>
+      </c>
+      <c r="H26" s="1">
+        <f t="shared" si="4"/>
+        <v>-1.190648855055997</v>
+      </c>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="8:15" x14ac:dyDescent="0.35">
-      <c r="H27" s="1"/>
+    <row r="27" spans="6:12" x14ac:dyDescent="0.35">
+      <c r="F27" s="1">
+        <f t="shared" si="3"/>
+        <v>241.57482871319399</v>
+      </c>
+      <c r="G27" s="1">
+        <v>242.76547756824999</v>
+      </c>
+      <c r="H27" s="1">
+        <f t="shared" si="4"/>
+        <v>-1.190648855055997</v>
+      </c>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="8:15" x14ac:dyDescent="0.35">
-      <c r="H28" s="1"/>
+    <row r="28" spans="6:12" x14ac:dyDescent="0.35">
+      <c r="F28" s="1">
+        <f t="shared" si="3"/>
+        <v>241.57482871319399</v>
+      </c>
+      <c r="G28" s="1">
+        <v>242.195366069881</v>
+      </c>
+      <c r="H28" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.62053735668700938</v>
+      </c>
       <c r="L28" s="1"/>
+    </row>
+    <row r="29" spans="6:12" x14ac:dyDescent="0.35">
+      <c r="F29" s="1">
+        <f t="shared" si="3"/>
+        <v>241.57482871319399</v>
+      </c>
+      <c r="G29" s="1">
+        <v>242.57333738608901</v>
+      </c>
+      <c r="H29" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.99850867289501366</v>
+      </c>
+    </row>
+    <row r="30" spans="6:12" x14ac:dyDescent="0.35">
+      <c r="F30" s="1">
+        <f t="shared" si="3"/>
+        <v>241.57482871319399</v>
+      </c>
+      <c r="G30" s="1">
+        <v>242.76547756824999</v>
+      </c>
+      <c r="H30" s="1">
+        <f t="shared" si="4"/>
+        <v>-1.190648855055997</v>
+      </c>
+    </row>
+    <row r="31" spans="6:12" x14ac:dyDescent="0.35">
+      <c r="F31" s="1">
+        <f t="shared" si="3"/>
+        <v>241.57482871319399</v>
+      </c>
+      <c r="G31" s="1">
+        <v>242.54292390406101</v>
+      </c>
+      <c r="H31" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.96809519086701812</v>
+      </c>
+    </row>
+    <row r="32" spans="6:12" x14ac:dyDescent="0.35">
+      <c r="F32" s="1">
+        <f t="shared" si="3"/>
+        <v>241.57482871319399</v>
+      </c>
+      <c r="G32" s="1">
+        <v>242.56311910085901</v>
+      </c>
+      <c r="H32" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.98829038766501753</v>
+      </c>
+    </row>
+    <row r="33" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="F33" s="1">
+        <f t="shared" si="3"/>
+        <v>241.57482871319399</v>
+      </c>
+      <c r="G33" s="1">
+        <v>242.56311910085901</v>
+      </c>
+      <c r="H33" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.98829038766501753</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>